<commit_message>
The Library has been converting to database library
</commit_message>
<xml_diff>
--- a/Connectors, Interconnects/Terminal Blocks - Headers, Plugs and Sockets/Parameters.xlsx
+++ b/Connectors, Interconnects/Terminal Blocks - Headers, Plugs and Sockets/Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium Designer Library\Connectors, Interconnects\Terminal Blocks - Headers, Plugs and Sockets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_Designer_Library\Connectors, Interconnects\Terminal Blocks - Headers, Plugs and Sockets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F001C1-FFFC-44A6-8B9E-3E59E4AD9093}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BA966B-1267-44E4-A471-977DD1401B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>

</xml_diff>